<commit_message>
Final Commit isA -Menna
</commit_message>
<xml_diff>
--- a/DataSource/LoginData.xlsx
+++ b/DataSource/LoginData.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @#$$%%</t>
   </si>
   <si>
     <t>password</t>
@@ -34,9 +31,6 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>menna.maged.mostafa@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -81,10 +75,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -387,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,50 +397,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>123456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="12$#@%*"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>